<commit_message>
diary rafael 2019-01-09 update
</commit_message>
<xml_diff>
--- a/diaries/diary-rafael-oliveira.xlsx
+++ b/diaries/diary-rafael-oliveira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SWE265\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730AAD6F-C4C8-4EC0-B913-1B2C0D9B2AD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917CC7C7-E0C0-4972-A681-310D0BC02CC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Environment set up for the class</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -249,9 +252,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -266,6 +266,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -597,24 +600,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A3" s="1"/>
@@ -642,7 +645,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1"/>
@@ -705,24 +708,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="14" customFormat="1" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="11">
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="10">
         <v>43474</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>0.8930555555555556</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
+      <c r="C10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="12" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated rafaels first diary entry with more information
</commit_message>
<xml_diff>
--- a/diaries/diary-rafael-oliveira.xlsx
+++ b/diaries/diary-rafael-oliveira.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SWE265\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917CC7C7-E0C0-4972-A681-310D0BC02CC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FA5BE0-B3EC-4B42-989A-12C3F58D3198}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -75,19 +75,22 @@
     <t>rafbel</t>
   </si>
   <si>
-    <t>Learned the importance of reverse engineering</t>
-  </si>
-  <si>
-    <t>Excited for future classes</t>
-  </si>
-  <si>
-    <t>To learn what I should expect from the course</t>
-  </si>
-  <si>
-    <t>Environment set up for the class</t>
-  </si>
-  <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>5:00 PM - 7:00 PM</t>
+  </si>
+  <si>
+    <t>To learn what I should expect from the course and check if I have everything I need</t>
+  </si>
+  <si>
+    <t>Environment set up for the class, formed groups, and learned the importance of reverse engineering</t>
+  </si>
+  <si>
+    <t>Excited for future classes and whatever else is to come!</t>
+  </si>
+  <si>
+    <t>Improving my ability to read and understand code feels like a higher priority now, now that I have seen how important it can be</t>
   </si>
 </sst>
 </file>
@@ -591,15 +594,15 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F16" sqref="F15:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="34.62890625" customWidth="1"/>
+    <col min="1" max="7" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -610,7 +613,7 @@
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -619,7 +622,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -628,7 +631,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -641,7 +644,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -654,7 +657,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -667,7 +670,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -676,7 +679,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -685,7 +688,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -708,15 +711,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="13" customFormat="1" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>43474</v>
       </c>
-      <c r="B10" s="11">
-        <v>0.8930555555555556</v>
+      <c r="B10" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>16</v>
@@ -725,13 +728,13 @@
         <v>17</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -740,7 +743,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -749,7 +752,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -758,7 +761,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -767,7 +770,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -776,7 +779,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -785,7 +788,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -794,7 +797,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -803,7 +806,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -812,7 +815,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -821,7 +824,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -830,7 +833,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -839,7 +842,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -848,7 +851,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -857,7 +860,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -866,7 +869,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -875,7 +878,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -884,7 +887,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -893,7 +896,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -902,7 +905,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -911,7 +914,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -920,7 +923,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -929,7 +932,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -938,7 +941,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -947,7 +950,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -956,7 +959,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -965,7 +968,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -974,7 +977,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -983,7 +986,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -992,7 +995,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1001,7 +1004,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1010,7 +1013,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1019,7 +1022,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1028,7 +1031,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1037,7 +1040,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1046,7 +1049,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1055,7 +1058,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1064,7 +1067,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1073,7 +1076,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1082,7 +1085,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1091,7 +1094,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1100,7 +1103,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1109,7 +1112,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1118,7 +1121,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1127,7 +1130,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1136,7 +1139,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1145,7 +1148,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1154,7 +1157,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1163,7 +1166,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1172,7 +1175,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1181,7 +1184,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1190,7 +1193,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1199,7 +1202,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1208,7 +1211,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1217,7 +1220,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1226,7 +1229,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1235,7 +1238,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1244,7 +1247,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1253,7 +1256,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1262,7 +1265,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1271,7 +1274,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1280,7 +1283,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1289,7 +1292,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1298,7 +1301,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1307,7 +1310,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1316,7 +1319,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1325,7 +1328,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1334,7 +1337,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1343,7 +1346,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1352,7 +1355,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1361,7 +1364,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1370,7 +1373,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1379,7 +1382,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1388,7 +1391,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1397,7 +1400,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1406,7 +1409,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1415,7 +1418,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1424,7 +1427,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1433,7 +1436,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1442,7 +1445,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1451,7 +1454,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1460,7 +1463,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1469,7 +1472,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1478,7 +1481,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1487,7 +1490,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1496,7 +1499,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1505,7 +1508,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1514,7 +1517,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -1523,7 +1526,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -1532,7 +1535,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -1541,7 +1544,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -1550,7 +1553,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -1559,7 +1562,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -1568,7 +1571,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -1577,7 +1580,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -1586,7 +1589,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -1595,7 +1598,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -1604,7 +1607,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -1613,7 +1616,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -1622,7 +1625,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -1631,7 +1634,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -1640,7 +1643,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -1649,7 +1652,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -1658,7 +1661,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -1667,7 +1670,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -1676,7 +1679,7 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -1685,7 +1688,7 @@
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -1694,7 +1697,7 @@
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -1703,7 +1706,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -1712,7 +1715,7 @@
       <c r="F119" s="7"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -1721,7 +1724,7 @@
       <c r="F120" s="7"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -1730,7 +1733,7 @@
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -1739,7 +1742,7 @@
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -1748,7 +1751,7 @@
       <c r="F123" s="7"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -1757,7 +1760,7 @@
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>

</xml_diff>

<commit_message>
rafaels diary entries for 2019-01-16
</commit_message>
<xml_diff>
--- a/diaries/diary-rafael-oliveira.xlsx
+++ b/diaries/diary-rafael-oliveira.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SWE265\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FA5BE0-B3EC-4B42-989A-12C3F58D3198}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA15D8C-97E6-48BB-9B6B-BFDCC4A1DBE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -78,9 +79,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>5:00 PM - 7:00 PM</t>
-  </si>
-  <si>
     <t>To learn what I should expect from the course and check if I have everything I need</t>
   </si>
   <si>
@@ -91,6 +89,39 @@
   </si>
   <si>
     <t>Improving my ability to read and understand code feels like a higher priority now, now that I have seen how important it can be</t>
+  </si>
+  <si>
+    <t>3:00 PM - 5:00 PM</t>
+  </si>
+  <si>
+    <t>To decide which GitHub repository we will use for our class project</t>
+  </si>
+  <si>
+    <t>Nervous about the amount of work</t>
+  </si>
+  <si>
+    <t>There is a lot of projects out there, and a lot of them I actually have the necessary skills to contribute.</t>
+  </si>
+  <si>
+    <t>Learn good techniques for breaking down code and understanding it</t>
+  </si>
+  <si>
+    <t>Still nervous about the amount of work</t>
+  </si>
+  <si>
+    <t>5:00 PM - 7:50 PM</t>
+  </si>
+  <si>
+    <t>Chris Zhang, Nicolas Grantham, and Hyun Jay Yang</t>
+  </si>
+  <si>
+    <t>Fixed a few bugs in the Pacman project with the help of the class, learned a few basic techniques for code understanding, and how a professional reads code at Google</t>
+  </si>
+  <si>
+    <t>We came up with a list of the projects that we are interested in and feel that we are able to contribute, and in the end decided to use JUnit5 for our project</t>
+  </si>
+  <si>
+    <t>Understanding code in big projects can be harder than it seems if you are unfamiliar with the domain</t>
   </si>
 </sst>
 </file>
@@ -229,7 +260,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -269,6 +300,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -593,36 +627,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F15:F16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="7" width="34.5703125" customWidth="1"/>
+    <col min="1" max="7" width="34.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-    </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -631,7 +665,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -644,7 +678,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -657,7 +691,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -670,7 +704,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -679,7 +713,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -688,7 +722,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -711,48 +745,76 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10">
         <v>43474</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="F10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="12" t="s">
+    </row>
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="10">
+        <v>43481</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="10">
+        <v>43481</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -761,7 +823,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -770,7 +832,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -779,7 +841,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -788,7 +850,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -797,7 +859,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -806,7 +868,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -815,7 +877,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -824,7 +886,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -833,7 +895,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -842,7 +904,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -851,7 +913,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -860,7 +922,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -869,7 +931,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -878,7 +940,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -887,7 +949,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -896,7 +958,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -905,7 +967,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -914,7 +976,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -923,7 +985,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -932,7 +994,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -941,7 +1003,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -950,7 +1012,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -959,7 +1021,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -968,7 +1030,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -977,7 +1039,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -986,7 +1048,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -995,7 +1057,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1004,7 +1066,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1013,7 +1075,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1022,7 +1084,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1031,7 +1093,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1040,7 +1102,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1049,7 +1111,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1058,7 +1120,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1067,7 +1129,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1076,7 +1138,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1085,7 +1147,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1094,7 +1156,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1103,7 +1165,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1112,7 +1174,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1121,7 +1183,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1130,7 +1192,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1139,7 +1201,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1148,7 +1210,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1157,7 +1219,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1166,7 +1228,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1175,7 +1237,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1184,7 +1246,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1193,7 +1255,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1202,7 +1264,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1211,7 +1273,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1220,7 +1282,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1229,7 +1291,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1238,7 +1300,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1247,7 +1309,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1256,7 +1318,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1265,7 +1327,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1274,7 +1336,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1283,7 +1345,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1292,7 +1354,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1301,7 +1363,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1310,7 +1372,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1319,7 +1381,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1328,7 +1390,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1337,7 +1399,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1346,7 +1408,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1355,7 +1417,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1364,7 +1426,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1373,7 +1435,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1382,7 +1444,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1391,7 +1453,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1400,7 +1462,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1409,7 +1471,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1418,7 +1480,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1427,7 +1489,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1436,7 +1498,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1445,7 +1507,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1454,7 +1516,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1463,7 +1525,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1472,7 +1534,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1481,7 +1543,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1490,7 +1552,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1499,7 +1561,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1508,7 +1570,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1517,7 +1579,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -1526,7 +1588,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -1535,7 +1597,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -1544,7 +1606,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -1553,7 +1615,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -1562,7 +1624,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -1571,7 +1633,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -1580,7 +1642,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -1589,7 +1651,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -1598,7 +1660,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -1607,7 +1669,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -1616,7 +1678,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -1625,7 +1687,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -1634,7 +1696,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -1643,7 +1705,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -1652,7 +1714,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -1661,7 +1723,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -1670,7 +1732,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -1679,7 +1741,7 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -1688,7 +1750,7 @@
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -1697,7 +1759,7 @@
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -1706,7 +1768,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -1715,7 +1777,7 @@
       <c r="F119" s="7"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -1724,7 +1786,7 @@
       <c r="F120" s="7"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -1733,7 +1795,7 @@
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -1742,7 +1804,7 @@
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -1751,7 +1813,7 @@
       <c r="F123" s="7"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -1760,7 +1822,7 @@
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>

</xml_diff>

<commit_message>
rafaels diary entries for 2019-01-16 (#66)
</commit_message>
<xml_diff>
--- a/diaries/diary-rafael-oliveira.xlsx
+++ b/diaries/diary-rafael-oliveira.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SWE265\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FA5BE0-B3EC-4B42-989A-12C3F58D3198}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA15D8C-97E6-48BB-9B6B-BFDCC4A1DBE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -78,9 +79,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>5:00 PM - 7:00 PM</t>
-  </si>
-  <si>
     <t>To learn what I should expect from the course and check if I have everything I need</t>
   </si>
   <si>
@@ -91,6 +89,39 @@
   </si>
   <si>
     <t>Improving my ability to read and understand code feels like a higher priority now, now that I have seen how important it can be</t>
+  </si>
+  <si>
+    <t>3:00 PM - 5:00 PM</t>
+  </si>
+  <si>
+    <t>To decide which GitHub repository we will use for our class project</t>
+  </si>
+  <si>
+    <t>Nervous about the amount of work</t>
+  </si>
+  <si>
+    <t>There is a lot of projects out there, and a lot of them I actually have the necessary skills to contribute.</t>
+  </si>
+  <si>
+    <t>Learn good techniques for breaking down code and understanding it</t>
+  </si>
+  <si>
+    <t>Still nervous about the amount of work</t>
+  </si>
+  <si>
+    <t>5:00 PM - 7:50 PM</t>
+  </si>
+  <si>
+    <t>Chris Zhang, Nicolas Grantham, and Hyun Jay Yang</t>
+  </si>
+  <si>
+    <t>Fixed a few bugs in the Pacman project with the help of the class, learned a few basic techniques for code understanding, and how a professional reads code at Google</t>
+  </si>
+  <si>
+    <t>We came up with a list of the projects that we are interested in and feel that we are able to contribute, and in the end decided to use JUnit5 for our project</t>
+  </si>
+  <si>
+    <t>Understanding code in big projects can be harder than it seems if you are unfamiliar with the domain</t>
   </si>
 </sst>
 </file>
@@ -229,7 +260,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -269,6 +300,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -593,36 +627,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F15:F16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="7" width="34.5703125" customWidth="1"/>
+    <col min="1" max="7" width="34.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-    </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -631,7 +665,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -644,7 +678,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -657,7 +691,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -670,7 +704,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -679,7 +713,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -688,7 +722,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -711,48 +745,76 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10">
         <v>43474</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="F10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="12" t="s">
+    </row>
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="10">
+        <v>43481</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="10">
+        <v>43481</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -761,7 +823,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -770,7 +832,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -779,7 +841,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -788,7 +850,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -797,7 +859,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -806,7 +868,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -815,7 +877,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -824,7 +886,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -833,7 +895,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -842,7 +904,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -851,7 +913,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -860,7 +922,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -869,7 +931,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -878,7 +940,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -887,7 +949,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -896,7 +958,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -905,7 +967,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -914,7 +976,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -923,7 +985,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -932,7 +994,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -941,7 +1003,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -950,7 +1012,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -959,7 +1021,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -968,7 +1030,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -977,7 +1039,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -986,7 +1048,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -995,7 +1057,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1004,7 +1066,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1013,7 +1075,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1022,7 +1084,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1031,7 +1093,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1040,7 +1102,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1049,7 +1111,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1058,7 +1120,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1067,7 +1129,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1076,7 +1138,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1085,7 +1147,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1094,7 +1156,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1103,7 +1165,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1112,7 +1174,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1121,7 +1183,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1130,7 +1192,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1139,7 +1201,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1148,7 +1210,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1157,7 +1219,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1166,7 +1228,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1175,7 +1237,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1184,7 +1246,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1193,7 +1255,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1202,7 +1264,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1211,7 +1273,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1220,7 +1282,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1229,7 +1291,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1238,7 +1300,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1247,7 +1309,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1256,7 +1318,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1265,7 +1327,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1274,7 +1336,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1283,7 +1345,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1292,7 +1354,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1301,7 +1363,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1310,7 +1372,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1319,7 +1381,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1328,7 +1390,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1337,7 +1399,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1346,7 +1408,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1355,7 +1417,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1364,7 +1426,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1373,7 +1435,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1382,7 +1444,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1391,7 +1453,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1400,7 +1462,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1409,7 +1471,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1418,7 +1480,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1427,7 +1489,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1436,7 +1498,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1445,7 +1507,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1454,7 +1516,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1463,7 +1525,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1472,7 +1534,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1481,7 +1543,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1490,7 +1552,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1499,7 +1561,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1508,7 +1570,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1517,7 +1579,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -1526,7 +1588,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -1535,7 +1597,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -1544,7 +1606,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -1553,7 +1615,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -1562,7 +1624,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -1571,7 +1633,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -1580,7 +1642,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -1589,7 +1651,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -1598,7 +1660,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -1607,7 +1669,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -1616,7 +1678,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -1625,7 +1687,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -1634,7 +1696,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -1643,7 +1705,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -1652,7 +1714,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -1661,7 +1723,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -1670,7 +1732,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -1679,7 +1741,7 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -1688,7 +1750,7 @@
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -1697,7 +1759,7 @@
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -1706,7 +1768,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -1715,7 +1777,7 @@
       <c r="F119" s="7"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -1724,7 +1786,7 @@
       <c r="F120" s="7"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -1733,7 +1795,7 @@
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -1742,7 +1804,7 @@
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -1751,7 +1813,7 @@
       <c r="F123" s="7"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -1760,7 +1822,7 @@
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>

</xml_diff>

<commit_message>
Rafael's Diary 2019 01 18 (#100)
* rafaels diary entries for 2019-01-16

* diary entry 2019-01-18
</commit_message>
<xml_diff>
--- a/diaries/diary-rafael-oliveira.xlsx
+++ b/diaries/diary-rafael-oliveira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SWE265\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA15D8C-97E6-48BB-9B6B-BFDCC4A1DBE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA3D4EF-6917-4659-A052-97A73AA61EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -122,6 +121,21 @@
   </si>
   <si>
     <t>Understanding code in big projects can be harder than it seems if you are unfamiliar with the domain</t>
+  </si>
+  <si>
+    <t>9:05 - 10:35 AM</t>
+  </si>
+  <si>
+    <t>Understand and document all the code associated with the PacMan homework questions</t>
+  </si>
+  <si>
+    <t>Able to fully understand the parts of the code associated with the homework assignment</t>
+  </si>
+  <si>
+    <t>Feeling good overall</t>
+  </si>
+  <si>
+    <t>I am very thankful for my IDE's search tool. It really comes in handy when I need to look for specific keywords that might point me to the right direction</t>
   </si>
 </sst>
 </file>
@@ -627,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -814,14 +828,28 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="10">
+        <v>43483</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A14" s="7"/>

</xml_diff>

<commit_message>
rafael oliveira diary 2019-01-23
</commit_message>
<xml_diff>
--- a/diaries/diary-rafael-oliveira.xlsx
+++ b/diaries/diary-rafael-oliveira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SWE265\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA3D4EF-6917-4659-A052-97A73AA61EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4093A1-3B8E-4E1D-A9C3-6722A46D6EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -136,6 +136,36 @@
   </si>
   <si>
     <t>I am very thankful for my IDE's search tool. It really comes in handy when I need to look for specific keywords that might point me to the right direction</t>
+  </si>
+  <si>
+    <t>11:00 AM - 12:15 PM</t>
+  </si>
+  <si>
+    <t>Read all the study material included in the homework assignment</t>
+  </si>
+  <si>
+    <t>Better idea of how to approach big projects that I haven't seen before</t>
+  </si>
+  <si>
+    <t>Most techniques involve having an approach to a starting point and from there progressing on to the rest of the code</t>
+  </si>
+  <si>
+    <t>Looking forward to applying these concepts pratically</t>
+  </si>
+  <si>
+    <t>5:00 - 7:50 PM</t>
+  </si>
+  <si>
+    <t>Learned how to use UML as a visual tool to help understanding code and how to use the simpleUML plugin</t>
+  </si>
+  <si>
+    <t>Since I understand things better when I see them, visual tools can help me a lot when used</t>
+  </si>
+  <si>
+    <t>Nervous about the amount of homework</t>
+  </si>
+  <si>
+    <t>Acquire new techniques to understand code in a simplified manner</t>
   </si>
 </sst>
 </file>
@@ -274,7 +304,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -320,6 +350,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -641,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -761,7 +794,7 @@
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10">
-        <v>43474</v>
+        <v>43839</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>25</v>
@@ -784,7 +817,7 @@
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10">
-        <v>43481</v>
+        <v>43846</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>19</v>
@@ -807,7 +840,7 @@
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="10">
-        <v>43481</v>
+        <v>43846</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>25</v>
@@ -830,7 +863,7 @@
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10">
-        <v>43483</v>
+        <v>43848</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>30</v>
@@ -851,86 +884,114 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8"/>
+    <row r="14" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="10">
+        <v>43852</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="13" customFormat="1" ht="46.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="10">
+        <v>44158</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A23" s="7"/>

</xml_diff>

<commit_message>
rafael oliveiras diary update 2020-01-26
</commit_message>
<xml_diff>
--- a/diaries/diary-rafael-oliveira.xlsx
+++ b/diaries/diary-rafael-oliveira.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SWE265\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4093A1-3B8E-4E1D-A9C3-6722A46D6EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC2ED3F-D1F5-48E4-A869-8101A7238773}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -166,6 +166,21 @@
   </si>
   <si>
     <t>Acquire new techniques to understand code in a simplified manner</t>
+  </si>
+  <si>
+    <t>Finish all the tasks from the first project assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracted the UML diagram from our project, choose two features, and documented how we found those features using code reading techniques, </t>
+  </si>
+  <si>
+    <t>UML helps me a lot as a visual tool, but if it is a huge diagram, I have to break it up in parts so I can work with a smaller scope that might be easier to understand. On the other hand, the templates provided during class confuse me, but I am trying to see if I can get used to them</t>
+  </si>
+  <si>
+    <t>Tired from the amount of work, but proud of my group for what we accomplished so far</t>
+  </si>
+  <si>
+    <t>3:00 PM - 7:30 PM</t>
   </si>
 </sst>
 </file>
@@ -348,11 +363,11 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -674,36 +689,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="34.578125" customWidth="1"/>
+    <col min="1" max="7" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -712,7 +727,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -725,7 +740,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -738,7 +753,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -751,7 +766,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -760,7 +775,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -769,7 +784,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -792,7 +807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>43839</v>
       </c>
@@ -815,7 +830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>43846</v>
       </c>
@@ -838,7 +853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>43846</v>
       </c>
@@ -861,7 +876,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>43848</v>
       </c>
@@ -884,7 +899,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>43852</v>
       </c>
@@ -907,9 +922,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="13" customFormat="1" ht="46.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
-        <v>44158</v>
+        <v>43853</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>40</v>
@@ -930,34 +945,48 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>43855</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="16"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -966,7 +995,7 @@
       <c r="F19" s="12"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -975,7 +1004,7 @@
       <c r="F20" s="12"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -984,7 +1013,7 @@
       <c r="F21" s="12"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -993,7 +1022,7 @@
       <c r="F22" s="12"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1002,7 +1031,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1011,7 +1040,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1020,7 +1049,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1029,7 +1058,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1038,7 +1067,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1047,7 +1076,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1056,7 +1085,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1065,7 +1094,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1074,7 +1103,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1083,7 +1112,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1092,7 +1121,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1101,7 +1130,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1110,7 +1139,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1119,7 +1148,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1128,7 +1157,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1137,7 +1166,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1146,7 +1175,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1155,7 +1184,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1164,7 +1193,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1173,7 +1202,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1182,7 +1211,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1191,7 +1220,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1200,7 +1229,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1209,7 +1238,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1218,7 +1247,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1227,7 +1256,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1236,7 +1265,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1245,7 +1274,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1254,7 +1283,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1263,7 +1292,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1272,7 +1301,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1281,7 +1310,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1290,7 +1319,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1299,7 +1328,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1308,7 +1337,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1317,7 +1346,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1326,7 +1355,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1335,7 +1364,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1344,7 +1373,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1353,7 +1382,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1362,7 +1391,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1371,7 +1400,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1380,7 +1409,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1389,7 +1418,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1398,7 +1427,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1407,7 +1436,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1416,7 +1445,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1425,7 +1454,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1434,7 +1463,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1443,7 +1472,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1452,7 +1481,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1461,7 +1490,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1470,7 +1499,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1479,7 +1508,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1488,7 +1517,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1497,7 +1526,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1506,7 +1535,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1515,7 +1544,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1524,7 +1553,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1533,7 +1562,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1542,7 +1571,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1551,7 +1580,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1560,7 +1589,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1569,7 +1598,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1578,7 +1607,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1587,7 +1616,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1596,7 +1625,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1605,7 +1634,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1614,7 +1643,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1623,7 +1652,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1632,7 +1661,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1641,7 +1670,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1650,7 +1679,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1659,7 +1688,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1668,7 +1697,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -1677,7 +1706,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -1686,7 +1715,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -1695,7 +1724,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -1704,7 +1733,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -1713,7 +1742,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -1722,7 +1751,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -1731,7 +1760,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -1740,7 +1769,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -1749,7 +1778,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -1758,7 +1787,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -1767,7 +1796,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -1776,7 +1805,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -1785,7 +1814,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -1794,7 +1823,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -1803,7 +1832,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -1812,7 +1841,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -1821,7 +1850,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -1830,7 +1859,7 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -1839,7 +1868,7 @@
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -1848,7 +1877,7 @@
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -1857,7 +1886,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -1866,7 +1895,7 @@
       <c r="F119" s="7"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -1875,7 +1904,7 @@
       <c r="F120" s="7"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -1884,7 +1913,7 @@
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -1893,7 +1922,7 @@
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -1902,7 +1931,7 @@
       <c r="F123" s="7"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -1911,7 +1940,7 @@
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>

</xml_diff>

<commit_message>
updated rafaels diary from 2020-02-06 to 2020-02-16
</commit_message>
<xml_diff>
--- a/diaries/diary-rafael-oliveira.xlsx
+++ b/diaries/diary-rafael-oliveira.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SWE265\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A365CE19-3DA6-4FB2-825F-FC8FAAEDC69B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7C1A60-58EF-47D4-9300-801C0B87913D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -220,6 +220,63 @@
   </si>
   <si>
     <t>The guest speaker was honest about the industry really is. Also, it is very hard to externalize your mental model if others have a different way to approach code</t>
+  </si>
+  <si>
+    <t>7:00 PM - 7:50 PM</t>
+  </si>
+  <si>
+    <t>Learn more about key roles and key people in our project structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understanding who are the core maintainers in a system can be key if we can establish contact with them and ask them for help </t>
+  </si>
+  <si>
+    <t>Tired from the midterm, but ready for whatever comes next</t>
+  </si>
+  <si>
+    <t>Learned more about how stakeholders and key developers influence and are influenced by a system. Also learned how to better analyze a system's functionality</t>
+  </si>
+  <si>
+    <t>Tired, but feeling good overall</t>
+  </si>
+  <si>
+    <t>8:00 PM - 8:20 PM</t>
+  </si>
+  <si>
+    <t>Identify our system's functionality, stakeholders, and key developers</t>
+  </si>
+  <si>
+    <t>6:30PM - 7:30 PM</t>
+  </si>
+  <si>
+    <t>3:00PM - 6:30 PM</t>
+  </si>
+  <si>
+    <t>Identify a new essential feature for assignment 2</t>
+  </si>
+  <si>
+    <t>Identified the map generator feature, and able to map about how it works</t>
+  </si>
+  <si>
+    <t>This feature seems more essential than the save feature, maybe I understand better what an essential feature is now</t>
+  </si>
+  <si>
+    <t>Feeling good, but tired</t>
+  </si>
+  <si>
+    <t>Identified all we needed for assignment 3, but the non-functional aspects of FreeCol (our project)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By organizing key developers into different groups, we have a better notion of who we should ask for help when we need help </t>
+  </si>
+  <si>
+    <t>Organize when we should meet and what should we do</t>
+  </si>
+  <si>
+    <t>Finding stakeholder information is not as easy as it seems, but key developers can be easy if they are directly linked to the project in a website</t>
+  </si>
+  <si>
+    <t>Decided when we should meet and what we should do those days</t>
   </si>
 </sst>
 </file>
@@ -358,7 +415,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -404,6 +461,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -725,16 +785,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="34.578125" customWidth="1"/>
+    <col min="1" max="7" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -745,7 +805,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -754,7 +814,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -763,7 +823,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -776,7 +836,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -789,7 +849,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -802,7 +862,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -811,7 +871,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -820,7 +880,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -843,7 +903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>43839</v>
       </c>
@@ -866,7 +926,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>43846</v>
       </c>
@@ -889,7 +949,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>43846</v>
       </c>
@@ -912,7 +972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>43848</v>
       </c>
@@ -935,7 +995,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>43852</v>
       </c>
@@ -958,7 +1018,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="13" customFormat="1" ht="46.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>43853</v>
       </c>
@@ -981,7 +1041,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" ht="124.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>43855</v>
       </c>
@@ -1004,7 +1064,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="13" customFormat="1" ht="46.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>43860</v>
       </c>
@@ -1027,7 +1087,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" s="13" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>43862</v>
       </c>
@@ -1050,9 +1110,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
-        <v>43983</v>
+        <v>43867</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>59</v>
@@ -1073,43 +1133,99 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>43874</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>43874</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>43877</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>43877</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1118,7 +1234,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1127,7 +1243,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1136,7 +1252,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1145,7 +1261,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1154,7 +1270,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1163,7 +1279,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1172,7 +1288,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1181,7 +1297,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1190,7 +1306,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1199,7 +1315,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1208,7 +1324,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1217,7 +1333,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1226,7 +1342,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1235,7 +1351,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1244,7 +1360,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1253,7 +1369,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1262,7 +1378,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1271,7 +1387,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1280,7 +1396,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1289,7 +1405,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1298,7 +1414,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1307,7 +1423,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1316,7 +1432,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1325,7 +1441,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1334,7 +1450,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1343,7 +1459,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1352,7 +1468,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1361,7 +1477,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1370,7 +1486,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1379,7 +1495,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1388,7 +1504,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1397,7 +1513,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1406,7 +1522,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1415,7 +1531,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1424,7 +1540,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1433,7 +1549,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1442,7 +1558,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1451,7 +1567,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1460,7 +1576,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1469,7 +1585,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1478,7 +1594,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1487,7 +1603,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1496,7 +1612,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1505,7 +1621,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1514,7 +1630,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1523,7 +1639,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1532,7 +1648,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1541,7 +1657,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1550,7 +1666,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1559,7 +1675,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1568,7 +1684,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1577,7 +1693,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1586,7 +1702,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1595,7 +1711,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1604,7 +1720,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1613,7 +1729,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1622,7 +1738,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1631,7 +1747,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1640,7 +1756,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1649,7 +1765,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1658,7 +1774,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1667,7 +1783,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1676,7 +1792,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1685,7 +1801,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1694,7 +1810,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1703,7 +1819,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1712,7 +1828,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1721,7 +1837,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1730,7 +1846,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1739,7 +1855,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1748,7 +1864,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1757,7 +1873,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1766,7 +1882,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1775,7 +1891,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -1784,7 +1900,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -1793,7 +1909,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -1802,7 +1918,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -1811,7 +1927,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -1820,7 +1936,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -1829,7 +1945,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -1838,7 +1954,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -1847,7 +1963,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -1856,7 +1972,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -1865,7 +1981,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -1874,7 +1990,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -1883,7 +1999,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -1892,7 +2008,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -1901,7 +2017,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -1910,7 +2026,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -1919,7 +2035,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -1928,7 +2044,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -1937,7 +2053,7 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -1946,7 +2062,7 @@
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -1955,7 +2071,7 @@
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -1964,7 +2080,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -1973,7 +2089,7 @@
       <c r="F119" s="7"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -1982,7 +2098,7 @@
       <c r="F120" s="7"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -1991,7 +2107,7 @@
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -2000,7 +2116,7 @@
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -2009,7 +2125,7 @@
       <c r="F123" s="7"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -2018,7 +2134,7 @@
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>

</xml_diff>

<commit_message>
rafaels diary update 2020-02-23 (#385)
</commit_message>
<xml_diff>
--- a/diaries/diary-rafael-oliveira.xlsx
+++ b/diaries/diary-rafael-oliveira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7C1A60-58EF-47D4-9300-801C0B87913D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689D4776-FBAB-437D-AF78-9EA8E6381A97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -277,6 +277,48 @@
   </si>
   <si>
     <t>Decided when we should meet and what we should do those days</t>
+  </si>
+  <si>
+    <t>2:30PM - 5:00 PM</t>
+  </si>
+  <si>
+    <t>Finish and resubmit assignment 2</t>
+  </si>
+  <si>
+    <t>We rewrote the document using higher level abstractions and went our discovery process more throughly</t>
+  </si>
+  <si>
+    <t>Structuring the document into paragraphs and making links to our diagrams makes our document more understandable</t>
+  </si>
+  <si>
+    <t>2:00PM - 7:10 PM</t>
+  </si>
+  <si>
+    <t>Exhausted</t>
+  </si>
+  <si>
+    <t>Explained the social context, identified interesting pull requests and issues, and explained the architecture of our project in a concise document</t>
+  </si>
+  <si>
+    <t>Finish and deliver our project assignment #4</t>
+  </si>
+  <si>
+    <t>Since we had already worked on the essential features, we already had a general understanding of our project, so it was easier to understand the architecture because we knew the exact routes we had to study</t>
+  </si>
+  <si>
+    <t>5:00PM - 7:00 PM</t>
+  </si>
+  <si>
+    <t>Learn new expert key practices, what is social context, and how does architecture can help understanding code</t>
+  </si>
+  <si>
+    <t>Understood what social context is and how it might affect our decisions when choosing a project, and  how professionals use architecture as a comprehension tool</t>
+  </si>
+  <si>
+    <t>Feeling ok</t>
+  </si>
+  <si>
+    <t>It was good to hear our guest speakers give suggestions on how to introduce new members to the project and team, and how they guide them in the proper way to contribute</t>
   </si>
 </sst>
 </file>
@@ -459,11 +501,11 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -785,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,24 +837,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1215,42 +1257,84 @@
       <c r="D23" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="15" t="s">
         <v>75</v>
       </c>
       <c r="G23" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
+    <row r="24" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>43880</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>43881</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>43882</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>

</xml_diff>

<commit_message>
rafaels diary entries up to 2020-03-14
</commit_message>
<xml_diff>
--- a/diaries/diary-rafael-oliveira.xlsx
+++ b/diaries/diary-rafael-oliveira.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\W2020\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SWE265\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23207950-34A2-4246-B105-067229C8D391}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F354F7D-6D92-4F06-AD2A-8AD1848C2D77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="117">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -346,6 +346,42 @@
   </si>
   <si>
     <t>Since we had previous knowledge of the system, working on a bug took less time than it usually takes when you are handed a project for the first time. It also helps that it was not the first time we were seeing what our project is supposed to do</t>
+  </si>
+  <si>
+    <t>Test cases can show us through a input, output format what we should expect from certain parts of the code. If we map that information and associate it with domain knowledge we can learn valuable insight.</t>
+  </si>
+  <si>
+    <t>Understand how test cases can help us understand code</t>
+  </si>
+  <si>
+    <t>Learned new key expert practices and how test cases can be useful to actually understand how the code is supposed to behave</t>
+  </si>
+  <si>
+    <t>Feeling good, but a bit tired</t>
+  </si>
+  <si>
+    <t>2:00PM - 7:00 PM</t>
+  </si>
+  <si>
+    <t>Learn advanced topics</t>
+  </si>
+  <si>
+    <t>Learned new key expert practices, how the history of the project can be relevant, and how visualizations can offer good insight</t>
+  </si>
+  <si>
+    <t>Even after the program is over, I must keep studying to stay up to date with the current trends. This way I am almost always ready for what is coming</t>
+  </si>
+  <si>
+    <t>Finish the last assignment for the class</t>
+  </si>
+  <si>
+    <t>Contributed with our second issue, studying and detailed three test cases that we found interesting, and created new test cases for our project</t>
+  </si>
+  <si>
+    <t>Having good knowledge of the data-flow, control-flow, and architecture of our project made our contribution so much easier, since we knew what had to be changed, making the code understanding part of the assignment easier.</t>
+  </si>
+  <si>
+    <t>Feeling tired, but glad to have contributed</t>
   </si>
 </sst>
 </file>
@@ -854,16 +890,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="7" width="34.5703125" customWidth="1"/>
+    <col min="1" max="7" width="34.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -874,7 +910,7 @@
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -883,7 +919,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -892,7 +928,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -905,7 +941,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -918,7 +954,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -931,7 +967,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -940,7 +976,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -949,7 +985,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -972,7 +1008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10">
         <v>43839</v>
       </c>
@@ -995,7 +1031,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10">
         <v>43846</v>
       </c>
@@ -1018,7 +1054,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="10">
         <v>43846</v>
       </c>
@@ -1041,7 +1077,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10">
         <v>43848</v>
       </c>
@@ -1064,7 +1100,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10">
         <v>43852</v>
       </c>
@@ -1087,7 +1123,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="13" customFormat="1" ht="46.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="10">
         <v>43853</v>
       </c>
@@ -1110,7 +1146,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="124.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10">
         <v>43855</v>
       </c>
@@ -1133,7 +1169,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="13" customFormat="1" ht="46.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10">
         <v>43860</v>
       </c>
@@ -1156,7 +1192,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="13" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10">
         <v>43862</v>
       </c>
@@ -1179,7 +1215,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="10">
         <v>43867</v>
       </c>
@@ -1202,7 +1238,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="10">
         <v>43874</v>
       </c>
@@ -1225,7 +1261,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="13" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="13" customFormat="1" ht="78" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="10">
         <v>43874</v>
       </c>
@@ -1248,7 +1284,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="13" customFormat="1" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="10">
         <v>43877</v>
       </c>
@@ -1271,7 +1307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10">
         <v>43877</v>
       </c>
@@ -1294,7 +1330,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10">
         <v>43880</v>
       </c>
@@ -1317,7 +1353,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="78" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10">
         <v>43881</v>
       </c>
@@ -1340,7 +1376,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="93.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="10">
         <v>43882</v>
       </c>
@@ -1363,7 +1399,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="62.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10">
         <v>43887</v>
       </c>
@@ -1386,7 +1422,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="109.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="10">
         <v>43891</v>
       </c>
@@ -1409,34 +1445,76 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="93.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="10">
+        <v>43895</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="78" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="10">
+        <v>43902</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="109.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="10">
+        <v>43904</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1445,7 +1523,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1454,7 +1532,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1463,7 +1541,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1472,7 +1550,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1481,7 +1559,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1490,7 +1568,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1499,7 +1577,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1508,7 +1586,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1517,7 +1595,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1526,7 +1604,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1535,7 +1613,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1544,7 +1622,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1553,7 +1631,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1562,7 +1640,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1571,7 +1649,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1580,7 +1658,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1589,7 +1667,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1598,7 +1676,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1607,7 +1685,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1616,7 +1694,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1625,7 +1703,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1634,7 +1712,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1643,7 +1721,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1652,7 +1730,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1661,7 +1739,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1670,7 +1748,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1679,7 +1757,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1688,7 +1766,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1697,7 +1775,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1706,7 +1784,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1715,7 +1793,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1724,7 +1802,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1733,7 +1811,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1742,7 +1820,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1751,7 +1829,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1760,7 +1838,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1769,7 +1847,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1778,7 +1856,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1787,7 +1865,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1796,7 +1874,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1805,7 +1883,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1814,7 +1892,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1823,7 +1901,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1832,7 +1910,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1841,7 +1919,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1850,7 +1928,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1859,7 +1937,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1868,7 +1946,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1877,7 +1955,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1886,7 +1964,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1895,7 +1973,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1904,7 +1982,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1913,7 +1991,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1922,7 +2000,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1931,7 +2009,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1940,7 +2018,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1949,7 +2027,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1958,7 +2036,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1967,7 +2045,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1976,7 +2054,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1985,7 +2063,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1994,7 +2072,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -2003,7 +2081,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -2012,7 +2090,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -2021,7 +2099,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -2030,7 +2108,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -2039,7 +2117,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -2048,7 +2126,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -2057,7 +2135,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -2066,7 +2144,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -2075,7 +2153,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -2084,7 +2162,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -2093,7 +2171,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -2102,7 +2180,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -2111,7 +2189,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -2120,7 +2198,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -2129,7 +2207,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -2138,7 +2216,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -2147,7 +2225,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -2156,7 +2234,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -2165,7 +2243,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -2174,7 +2252,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -2183,7 +2261,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -2192,7 +2270,7 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -2201,7 +2279,7 @@
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -2210,7 +2288,7 @@
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -2219,7 +2297,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -2228,7 +2306,7 @@
       <c r="F119" s="7"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -2237,7 +2315,7 @@
       <c r="F120" s="7"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -2246,7 +2324,7 @@
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -2255,7 +2333,7 @@
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -2264,7 +2342,7 @@
       <c r="F123" s="7"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -2273,7 +2351,7 @@
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>

</xml_diff>